<commit_message>
Incorporated reading excel data to create book
</commit_message>
<xml_diff>
--- a/excelDataDrivenData.xlsx
+++ b/excelDataDrivenData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t xml:space="preserve">Testcases</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t xml:space="preserve">C4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AddBook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excel Driven Book</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isbnNum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maruf RA</t>
   </si>
 </sst>
 </file>
@@ -202,10 +214,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -223,6 +235,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -278,6 +293,23 @@
       </c>
       <c r="D5" s="1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>98761</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>